<commit_message>
Massedaten Neu mit 100 Kursen
</commit_message>
<xml_diff>
--- a/Massedaten.xlsx
+++ b/Massedaten.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenni\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99A2A143-FB3C-46A0-985D-8B7E2484F5D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A10E819-7325-48F8-8519-05C48FA1226B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$2:$K$102</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="100">
   <si>
     <t xml:space="preserve">Raum </t>
   </si>
@@ -126,9 +129,6 @@
     <t>Jennifer Ferle</t>
   </si>
   <si>
-    <t>Beginner, Fortgeschritten</t>
-  </si>
-  <si>
     <t>Fortgeschritten</t>
   </si>
   <si>
@@ -138,15 +138,9 @@
     <t>Expertise</t>
   </si>
   <si>
-    <t>Tanz, Gymnastik</t>
-  </si>
-  <si>
     <t>Kondition, Muskelaufbau</t>
   </si>
   <si>
-    <t>Kampfsport, Yoga, Muskelaufbau</t>
-  </si>
-  <si>
     <t>Schwimminstruktor, Muskelaufbau</t>
   </si>
   <si>
@@ -162,27 +156,6 @@
     <t>Equipment</t>
   </si>
   <si>
-    <t>Schwimmnudeln, Tauchringe</t>
-  </si>
-  <si>
-    <t>Hanteln, Yoga-Matten</t>
-  </si>
-  <si>
-    <t>Hanteln, Musikanlage, Yoga-Matten</t>
-  </si>
-  <si>
-    <t>Musikanlage, Schutzausrüstung, Yoga-Matten</t>
-  </si>
-  <si>
-    <t>Musikanlage, Yoga-Matten</t>
-  </si>
-  <si>
-    <t>Hanteln, Stepper, Musikanlage, Yoga-Matten</t>
-  </si>
-  <si>
-    <t>Gummibänder, Musikanlage, Yoga-Matten</t>
-  </si>
-  <si>
     <t>Geschlecht</t>
   </si>
   <si>
@@ -205,6 +178,156 @@
   </si>
   <si>
     <t>Jiu Jitsu</t>
+  </si>
+  <si>
+    <t>Beginne</t>
+  </si>
+  <si>
+    <t>Aikido</t>
+  </si>
+  <si>
+    <t>Badminton</t>
+  </si>
+  <si>
+    <t>Ballett</t>
+  </si>
+  <si>
+    <t>Beach Volleyball</t>
+  </si>
+  <si>
+    <t>Dance Aerobic</t>
+  </si>
+  <si>
+    <t>Figur Pur</t>
+  </si>
+  <si>
+    <t>Rücken Fit</t>
+  </si>
+  <si>
+    <t>Wirbelsäulengymnastik</t>
+  </si>
+  <si>
+    <t>TRX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bike Intense </t>
+  </si>
+  <si>
+    <t>Bike &amp; Climb</t>
+  </si>
+  <si>
+    <t>Powercore</t>
+  </si>
+  <si>
+    <t>BikeBasics</t>
+  </si>
+  <si>
+    <t>Fitness Running</t>
+  </si>
+  <si>
+    <t>Outdoor Circuit</t>
+  </si>
+  <si>
+    <t>Strong Back</t>
+  </si>
+  <si>
+    <t>BodyCombat</t>
+  </si>
+  <si>
+    <t>Crosstraining</t>
+  </si>
+  <si>
+    <t>Gymnastic</t>
+  </si>
+  <si>
+    <t>Float Yoga</t>
+  </si>
+  <si>
+    <t>Jumping Fitness</t>
+  </si>
+  <si>
+    <t>Aqua Running</t>
+  </si>
+  <si>
+    <t>Mommyfit</t>
+  </si>
+  <si>
+    <t>BodyPump</t>
+  </si>
+  <si>
+    <t>Hot Iron</t>
+  </si>
+  <si>
+    <t>Body Fight</t>
+  </si>
+  <si>
+    <t>Latino Dance</t>
+  </si>
+  <si>
+    <t>Tai Chi</t>
+  </si>
+  <si>
+    <t>Kettleball</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AthletiCore </t>
+  </si>
+  <si>
+    <t>Full Body Stretch</t>
+  </si>
+  <si>
+    <t>PowerCircle</t>
+  </si>
+  <si>
+    <t>Max Mustermann</t>
+  </si>
+  <si>
+    <t>Outdoor</t>
+  </si>
+  <si>
+    <t>Kampfsport, Entspannung, Muskelaufbau</t>
+  </si>
+  <si>
+    <t>Dirk Keller</t>
+  </si>
+  <si>
+    <t>Mark Blume</t>
+  </si>
+  <si>
+    <t>Ballsport, Muskelaufbau, Kondition</t>
+  </si>
+  <si>
+    <t>Entspannung, Stretching, Muskelaufbau</t>
+  </si>
+  <si>
+    <t>Tanz, Gymnastik, Kondition</t>
+  </si>
+  <si>
+    <t>Badminton-Schläger, Volleybälle, Outdoor-Hanteln</t>
+  </si>
+  <si>
+    <t>Yoga-Matten, Musikanlage, Hanteln, Langhanteln</t>
+  </si>
+  <si>
+    <t>Yoga-Matten, Musikanlage, Hanteln, Holz-Schwerter, TRX-Equipment, Ballett-Stange, Hanteln</t>
+  </si>
+  <si>
+    <t>Yoga-Matten, Musikanlage, Boxhandschuhe, Schutzkleidung, Sportfahrräder, Hanteln</t>
+  </si>
+  <si>
+    <t>Yoga-Matten, Musikanlage, Springseile, Stepper, Hanteln</t>
+  </si>
+  <si>
+    <t>Yoga-Matten, Musikanlage, Stepper, Gummibänder, Gymnastikbälle, Langhanteln, Gewichte</t>
+  </si>
+  <si>
+    <t>Yoga-Matten, Musikanlage, Kettle-Bälle, Gewichte, Hanteln, Langhanteln, Gymnastik-Bälle</t>
+  </si>
+  <si>
+    <t>Schwimmnudeln, Tauchringe, Gewichte</t>
+  </si>
+  <si>
+    <t>Biking, Kondition, Muskelaufbau</t>
   </si>
 </sst>
 </file>
@@ -228,7 +351,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -309,11 +432,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -324,6 +460,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -604,24 +743,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
     <col min="2" max="2" width="40.26953125" customWidth="1"/>
     <col min="3" max="3" width="20.26953125" customWidth="1"/>
     <col min="4" max="5" width="25.1796875" customWidth="1"/>
     <col min="6" max="6" width="26.1796875" customWidth="1"/>
     <col min="7" max="7" width="19.7265625" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" customWidth="1"/>
+    <col min="10" max="10" width="87.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -635,16 +776,25 @@
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -655,7 +805,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E3" s="9">
         <v>43466</v>
@@ -664,10 +814,19 @@
         <v>43525</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -678,7 +837,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E4" s="8">
         <v>43525</v>
@@ -687,10 +846,19 @@
         <v>43617</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -701,7 +869,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="9">
         <v>43497</v>
@@ -710,10 +878,19 @@
         <v>43586</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -724,7 +901,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E6" s="9">
         <v>43556</v>
@@ -733,10 +910,19 @@
         <v>43647</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -747,7 +933,7 @@
         <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E7" s="9">
         <v>43497</v>
@@ -756,10 +942,19 @@
         <v>43586</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -770,7 +965,7 @@
         <v>29</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E8" s="8">
         <v>43466</v>
@@ -779,10 +974,19 @@
         <v>43525</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -793,7 +997,7 @@
         <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E9" s="9">
         <v>43617</v>
@@ -802,10 +1006,19 @@
         <v>43709</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -816,7 +1029,7 @@
         <v>29</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E10" s="8">
         <v>43525</v>
@@ -825,10 +1038,10 @@
         <v>43617</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -839,7 +1052,7 @@
         <v>30</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E11" s="8">
         <v>43617</v>
@@ -848,10 +1061,16 @@
         <v>43709</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -862,7 +1081,7 @@
         <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="9">
         <v>43556</v>
@@ -871,10 +1090,16 @@
         <v>43647</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -885,7 +1110,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="9">
         <v>43525</v>
@@ -894,10 +1119,16 @@
         <v>43617</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -908,7 +1139,7 @@
         <v>32</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E14" s="8">
         <v>43647</v>
@@ -917,12 +1148,18 @@
         <v>43739</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>23</v>
@@ -931,7 +1168,7 @@
         <v>29</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="9">
         <v>43586</v>
@@ -940,10 +1177,16 @@
         <v>43678</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -954,7 +1197,7 @@
         <v>30</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" s="8">
         <v>43497</v>
@@ -963,10 +1206,16 @@
         <v>43586</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -977,7 +1226,7 @@
         <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E17" s="9">
         <v>43466</v>
@@ -986,10 +1235,16 @@
         <v>43525</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1000,7 +1255,7 @@
         <v>31</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E18" s="9">
         <v>43556</v>
@@ -1009,10 +1264,16 @@
         <v>43647</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1023,7 +1284,7 @@
         <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" s="9">
         <v>43497</v>
@@ -1032,10 +1293,16 @@
         <v>43586</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1046,7 +1313,7 @@
         <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E20" s="9">
         <v>43586</v>
@@ -1054,157 +1321,1920 @@
       <c r="F20" s="9">
         <v>43678</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="12"/>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="9">
+        <v>43466</v>
+      </c>
+      <c r="F21" s="8">
+        <v>43525</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="12"/>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="8">
+        <v>43525</v>
+      </c>
+      <c r="F22" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="9">
+        <v>43497</v>
+      </c>
+      <c r="F23" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="4" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="9">
+        <v>43556</v>
+      </c>
+      <c r="F24" s="9">
+        <v>43647</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="9">
+        <v>43497</v>
+      </c>
+      <c r="F25" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="8">
+        <v>43466</v>
+      </c>
+      <c r="F26" s="9">
+        <v>43525</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="9">
+        <v>43617</v>
+      </c>
+      <c r="F27" s="9">
+        <v>43709</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="8">
+        <v>43525</v>
+      </c>
+      <c r="F28" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="8">
+        <v>43617</v>
+      </c>
+      <c r="F29" s="9">
+        <v>43709</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="9">
+        <v>43556</v>
+      </c>
+      <c r="F30" s="9">
+        <v>43647</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="9">
+        <v>43525</v>
+      </c>
+      <c r="F31" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="8">
+        <v>43647</v>
+      </c>
+      <c r="F32" s="9">
+        <v>43739</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="9">
+        <v>43586</v>
+      </c>
+      <c r="F33" s="9">
+        <v>43678</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="8">
+        <v>43497</v>
+      </c>
+      <c r="F34" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="9">
+        <v>43466</v>
+      </c>
+      <c r="F35" s="9">
+        <v>43525</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="9">
+        <v>43556</v>
+      </c>
+      <c r="F36" s="9">
+        <v>43647</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="9">
+        <v>43497</v>
+      </c>
+      <c r="F37" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="9">
+        <v>43586</v>
+      </c>
+      <c r="F38" s="9">
+        <v>43678</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="9">
+        <v>43466</v>
+      </c>
+      <c r="F39" s="8">
+        <v>43525</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="B40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="8">
+        <v>43525</v>
+      </c>
+      <c r="F40" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="9">
+        <v>43497</v>
+      </c>
+      <c r="F41" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="9">
+        <v>43556</v>
+      </c>
+      <c r="F42" s="9">
+        <v>43647</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" s="9">
+        <v>43497</v>
+      </c>
+      <c r="F43" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="8">
+        <v>43466</v>
+      </c>
+      <c r="F44" s="9">
+        <v>43525</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" s="9">
+        <v>43617</v>
+      </c>
+      <c r="F45" s="9">
+        <v>43709</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E46" s="8">
+        <v>43525</v>
+      </c>
+      <c r="F46" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="8">
+        <v>43617</v>
+      </c>
+      <c r="F47" s="9">
+        <v>43709</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="9">
+        <v>43556</v>
+      </c>
+      <c r="F48" s="9">
+        <v>43647</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" s="9">
+        <v>43525</v>
+      </c>
+      <c r="F49" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="D50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E50" s="8">
+        <v>43647</v>
+      </c>
+      <c r="F50" s="9">
+        <v>43739</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E51" s="9">
+        <v>43586</v>
+      </c>
+      <c r="F51" s="9">
+        <v>43678</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" s="8">
+        <v>43497</v>
+      </c>
+      <c r="F52" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E53" s="9">
+        <v>43466</v>
+      </c>
+      <c r="F53" s="9">
+        <v>43525</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E54" s="9">
+        <v>43556</v>
+      </c>
+      <c r="F54" s="9">
+        <v>43647</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E55" s="9">
+        <v>43497</v>
+      </c>
+      <c r="F55" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" s="9">
+        <v>43586</v>
+      </c>
+      <c r="F56" s="9">
+        <v>43678</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57" s="9">
+        <v>43466</v>
+      </c>
+      <c r="F57" s="8">
+        <v>43525</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" s="8">
+        <v>43525</v>
+      </c>
+      <c r="F58" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E59" s="9">
+        <v>43497</v>
+      </c>
+      <c r="F59" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60" s="9">
+        <v>43556</v>
+      </c>
+      <c r="F60" s="9">
+        <v>43647</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E61" s="9">
+        <v>43497</v>
+      </c>
+      <c r="F61" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E62" s="8">
+        <v>43466</v>
+      </c>
+      <c r="F62" s="9">
+        <v>43525</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E63" s="9">
+        <v>43617</v>
+      </c>
+      <c r="F63" s="9">
+        <v>43709</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E64" s="8">
+        <v>43525</v>
+      </c>
+      <c r="F64" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E65" s="8">
+        <v>43617</v>
+      </c>
+      <c r="F65" s="9">
+        <v>43709</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E66" s="9">
+        <v>43556</v>
+      </c>
+      <c r="F66" s="9">
+        <v>43647</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E67" s="9">
+        <v>43525</v>
+      </c>
+      <c r="F67" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E68" s="8">
+        <v>43647</v>
+      </c>
+      <c r="F68" s="9">
+        <v>43739</v>
+      </c>
+      <c r="G68" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E69" s="9">
+        <v>43586</v>
+      </c>
+      <c r="F69" s="9">
+        <v>43678</v>
+      </c>
+      <c r="G69" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E70" s="8">
+        <v>43497</v>
+      </c>
+      <c r="F70" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G70" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E71" s="9">
+        <v>43466</v>
+      </c>
+      <c r="F71" s="9">
+        <v>43525</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E72" s="9">
+        <v>43556</v>
+      </c>
+      <c r="F72" s="9">
+        <v>43647</v>
+      </c>
+      <c r="G72" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="B73" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="D73" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E73" s="9">
+        <v>43497</v>
+      </c>
+      <c r="F73" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G73" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="B74" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E74" s="9">
+        <v>43586</v>
+      </c>
+      <c r="F74" s="9">
+        <v>43678</v>
+      </c>
+      <c r="G74" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E75" s="9">
+        <v>43466</v>
+      </c>
+      <c r="F75" s="8">
+        <v>43525</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="D76" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E76" s="8">
+        <v>43525</v>
+      </c>
+      <c r="F76" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="7" t="s">
+      <c r="D77" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E77" s="9">
+        <v>43497</v>
+      </c>
+      <c r="F77" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E78" s="9">
+        <v>43556</v>
+      </c>
+      <c r="F78" s="9">
+        <v>43647</v>
+      </c>
+      <c r="G78" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E79" s="9">
+        <v>43497</v>
+      </c>
+      <c r="F79" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E80" s="8">
+        <v>43466</v>
+      </c>
+      <c r="F80" s="9">
+        <v>43525</v>
+      </c>
+      <c r="G80" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E81" s="9">
+        <v>43617</v>
+      </c>
+      <c r="F81" s="9">
+        <v>43709</v>
+      </c>
+      <c r="G81" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E82" s="8">
+        <v>43525</v>
+      </c>
+      <c r="F82" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G82" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E83" s="8">
+        <v>43617</v>
+      </c>
+      <c r="F83" s="9">
+        <v>43709</v>
+      </c>
+      <c r="G83" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E84" s="9">
+        <v>43556</v>
+      </c>
+      <c r="F84" s="9">
+        <v>43647</v>
+      </c>
+      <c r="G84" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E85" s="9">
+        <v>43525</v>
+      </c>
+      <c r="F85" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G85" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E86" s="8">
+        <v>43647</v>
+      </c>
+      <c r="F86" s="9">
+        <v>43739</v>
+      </c>
+      <c r="G86" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E87" s="9">
+        <v>43586</v>
+      </c>
+      <c r="F87" s="9">
+        <v>43678</v>
+      </c>
+      <c r="G87" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E88" s="8">
+        <v>43497</v>
+      </c>
+      <c r="F88" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G88" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E89" s="9">
+        <v>43466</v>
+      </c>
+      <c r="F89" s="8">
+        <v>43525</v>
+      </c>
+      <c r="G89" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E90" s="8">
+        <v>43525</v>
+      </c>
+      <c r="F90" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G90" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E91" s="9">
+        <v>43497</v>
+      </c>
+      <c r="F91" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G91" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E92" s="9">
+        <v>43556</v>
+      </c>
+      <c r="F92" s="9">
+        <v>43647</v>
+      </c>
+      <c r="G92" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E93" s="9">
+        <v>43497</v>
+      </c>
+      <c r="F93" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G93" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
+      <c r="C94" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E94" s="8">
+        <v>43466</v>
+      </c>
+      <c r="F94" s="9">
+        <v>43525</v>
+      </c>
+      <c r="G94" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E95" s="9">
+        <v>43617</v>
+      </c>
+      <c r="F95" s="9">
+        <v>43709</v>
+      </c>
+      <c r="G95" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E96" s="8">
+        <v>43525</v>
+      </c>
+      <c r="F96" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E97" s="8">
+        <v>43617</v>
+      </c>
+      <c r="F97" s="9">
+        <v>43709</v>
+      </c>
+      <c r="G97" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E98" s="9">
+        <v>43556</v>
+      </c>
+      <c r="F98" s="9">
+        <v>43647</v>
+      </c>
+      <c r="G98" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E99" s="9">
+        <v>43525</v>
+      </c>
+      <c r="F99" s="9">
+        <v>43617</v>
+      </c>
+      <c r="G99" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E100" s="8">
+        <v>43647</v>
+      </c>
+      <c r="F100" s="9">
+        <v>43739</v>
+      </c>
+      <c r="G100" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>58</v>
+      <c r="C101" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E101" s="9">
+        <v>43586</v>
+      </c>
+      <c r="F101" s="9">
+        <v>43678</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E102" s="8">
+        <v>43497</v>
+      </c>
+      <c r="F102" s="9">
+        <v>43586</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:K102" xr:uid="{064F7E6E-ECC3-4666-9E1F-0CC369E02928}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>